<commit_message>
bug fixes on cases generator
</commit_message>
<xml_diff>
--- a/inputs/config.xlsx
+++ b/inputs/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pietro\Documents\git\loadshifting\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064CBDDD-E906-4EEC-A7C5-F9E8DFBD99FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F114B045-8825-4CCF-A465-CB54949529FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -1197,10 +1197,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
@@ -1500,8 +1496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2863,7 +2859,7 @@
       <formula>NOT(ISERROR(SEARCH("TRUE",D15)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations xWindow="587" yWindow="716" count="4">
+  <dataValidations xWindow="587" yWindow="716" count="3">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Valeur numérique" prompt="Introduire uniquement une valeur numérique!" sqref="D4:D6 D23:D25 D31:D36 D45:D50 D52:D54 D58:D61 D66 D69:D70 D72 D77:D80 D84:D93" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
@@ -2872,8 +2868,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Valeur numérique" prompt="Introduire uniquement une valeur numérique!" sqref="D95" xr:uid="{83E7BC87-6456-467A-84E8-F83989CBC5AE}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Valeur numérique" prompt="Introduire uniquement une valeur numérique!" sqref="D94" xr:uid="{0EB9596B-49ED-4E39-9F1E-C980982E38D7}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Valeur numérique" prompt="Introduire uniquement une valeur numérique!" sqref="D94:D95" xr:uid="{83E7BC87-6456-467A-84E8-F83989CBC5AE}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3129,8 +3124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>